<commit_message>
Issue with Parallel execution  of feature files
Issue with Parallel execution of feature files
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Excel_Login_Pythoncode.xlsx
+++ b/src/test/resources/TestData/Excel_Login_Pythoncode.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geeta\eclipse-workspace-2023\GitDesktop\DsAlgo_Scrutinizers_Prj\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F5C254-4D08-4787-AE96-637E469CC9D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16416497-F3C7-46FB-A6D2-BF2C4BE5D3D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14685" yWindow="3000" windowWidth="14115" windowHeight="13095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="LogIn" sheetId="1" r:id="rId1"/>
     <sheet name="pythonCode" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -450,7 +450,7 @@
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>